<commit_message>
updated the baja trip itinerary, although I am still waiting on confirmation from people from COBI and the cooperative on specific activities
</commit_message>
<xml_diff>
--- a/BajaTripItinerary.xlsx
+++ b/BajaTripItinerary.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Itinerary" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>Day</t>
   </si>
@@ -28,33 +29,15 @@
     <t>Leave Santa Barbara</t>
   </si>
   <si>
-    <t>Stop in San Diego to rest / lunch</t>
-  </si>
-  <si>
     <t>Arrive at El Rosario</t>
   </si>
   <si>
-    <t>Fast stop at UABC to pick up JCs degree (maybe)</t>
-  </si>
-  <si>
-    <t>Breakfast at Mama Espinoza</t>
-  </si>
-  <si>
     <t>Dinner with COBI at El Rosario (Mama Espinoza)</t>
   </si>
   <si>
     <t>Meet personnel from the coop and visit their fascilities</t>
   </si>
   <si>
-    <t>Lunch at Mama Espinoza</t>
-  </si>
-  <si>
-    <t>Pannel with fishers and members of the cooperative</t>
-  </si>
-  <si>
-    <t>Dinner at Mama Espinoza</t>
-  </si>
-  <si>
     <t>Travel to Punta Baja to go fishing with fishers</t>
   </si>
   <si>
@@ -80,6 +63,111 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>San Diego</t>
+  </si>
+  <si>
+    <t>Lunch at Ensenada</t>
+  </si>
+  <si>
+    <t>Depart to El Rosario</t>
+  </si>
+  <si>
+    <t>Actividad</t>
+  </si>
+  <si>
+    <t>Salida de Santa Barbara</t>
+  </si>
+  <si>
+    <t>Llegada a San Diego</t>
+  </si>
+  <si>
+    <t>Comida en Ensenada</t>
+  </si>
+  <si>
+    <t>Salida hacia El Rosario</t>
+  </si>
+  <si>
+    <t>Llegada a El Rosario</t>
+  </si>
+  <si>
+    <t>Cena con COBI en El Rosario (Mamá Espinoza)</t>
+  </si>
+  <si>
+    <t>Desayuno</t>
+  </si>
+  <si>
+    <t>Tour por la planta de El Rosario</t>
+  </si>
+  <si>
+    <t>Panel con miembros SCPP Ensenada</t>
+  </si>
+  <si>
+    <t>Pannel with members of the cooperative</t>
+  </si>
+  <si>
+    <t>Cena</t>
+  </si>
+  <si>
+    <t>Comida</t>
+  </si>
+  <si>
+    <t>Salida a Punta Baja para salir a pescar con miembros de la coop</t>
+  </si>
+  <si>
+    <t>Entrevistas</t>
+  </si>
+  <si>
+    <t>Perform surveys to fishers</t>
+  </si>
+  <si>
+    <t>Dinner</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>Salida de El Rosario</t>
+  </si>
+  <si>
+    <t>Ensenada</t>
+  </si>
+  <si>
+    <t>Cross the border in Tijuana</t>
+  </si>
+  <si>
+    <t>In San Diego</t>
+  </si>
+  <si>
+    <t>Arrive at SB</t>
+  </si>
+  <si>
+    <t>Comenzar a cruzar frontera</t>
+  </si>
+  <si>
+    <t>En San Diego</t>
+  </si>
+  <si>
+    <t>Llegada  SB</t>
+  </si>
+  <si>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>http://traffic.calit2.net/border/border-wait-times.php?type=pedestrian&amp;sub=standard&amp;port=250401</t>
+  </si>
+  <si>
+    <t>Wells Fargo</t>
+  </si>
+  <si>
+    <t>Antonio Muñoz Murillo</t>
+  </si>
+  <si>
+    <t>$292</t>
+  </si>
+  <si>
+    <t>motel@bajacactus.com</t>
   </si>
 </sst>
 </file>
@@ -95,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +193,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -121,11 +215,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,180 +517,391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.375" customWidth="1"/>
+    <col min="5" max="5" width="44.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
+      <c r="A1" s="5"/>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>42684</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="4">
+        <v>42685</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="5"/>
+      <c r="B12" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="5"/>
+      <c r="B13" s="3">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="5"/>
+      <c r="B14" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="5"/>
+      <c r="B15" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="4">
+        <v>42686</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="5"/>
+      <c r="B17" s="3">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="5"/>
+      <c r="B18" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="5"/>
+      <c r="B19" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="5"/>
+      <c r="B20" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1">
+        <v>42687</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>5969484723</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1">
         <v>42684</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="B3" s="2">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" s="2">
-        <v>0.625</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5" s="2">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" s="2">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1">
-        <v>42685</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8" s="2">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="B10" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="B11" s="2">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1">
-        <v>42686</v>
-      </c>
-      <c r="B12" s="3">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="B13" s="2">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="B14" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="B15" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1">
-        <v>42687</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="2"/>
-      <c r="C17" t="s">
-        <v>20</v>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>